<commit_message>
small change to form
</commit_message>
<xml_diff>
--- a/docs/IMR-SampleSubmissionSheet_v9(LASTNAME_MMMDD).xlsx
+++ b/docs/IMR-SampleSubmissionSheet_v9(LASTNAME_MMMDD).xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4069EA-3D27-4FAF-B3AF-AAE4BFE73494}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AD4E71-EC9E-461A-A03B-F51764691CE3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="742" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="149">
   <si>
     <t xml:space="preserve">Plate 1 </t>
   </si>
@@ -975,30 +975,6 @@
     <t>Put X below</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Use the color coding at left, and below right for mixtures, to color your samples in the plates below (using the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Format Painter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) if you are doing more than one target per submission. If only one target, put an X in the box of choice.</t>
-    </r>
-  </si>
-  <si>
     <t>BactV6/8+Arch</t>
   </si>
   <si>
@@ -1086,9 +1062,6 @@
     </r>
   </si>
   <si>
-    <t>Coming Oct.2018!</t>
-  </si>
-  <si>
     <t>Conc. (ng/µL)</t>
   </si>
   <si>
@@ -1099,6 +1072,36 @@
   </si>
   <si>
     <t>A260/230 ratio</t>
+  </si>
+  <si>
+    <t>(Not used for MiSeq!)</t>
+  </si>
+  <si>
+    <t>Coming Nov.2018!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Use the color coding at left, and below right for multiples, to color your samples in the plates below (using the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Format Painter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) if you are doing more than one target per submission. If only one target, put an X in the box of choice.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1703,7 +1706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1916,12 +1919,25 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1952,15 +1968,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1985,22 +1992,21 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2635,7 +2641,7 @@
     </row>
     <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="21" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -2667,7 +2673,7 @@
   <dimension ref="A1:AF78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:AA14"/>
+      <selection activeCell="I12" sqref="I12:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,20 +2682,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -2708,35 +2714,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="96"/>
-      <c r="J3" s="83" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
+      <c r="J3" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -2744,35 +2750,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="96"/>
-      <c r="J4" s="83" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="J4" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
-      <c r="X4" s="106"/>
-      <c r="Y4" s="106"/>
-      <c r="Z4" s="106"/>
-      <c r="AA4" s="106"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -2781,26 +2787,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="93" t="s">
+      <c r="J5" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="106"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -2808,30 +2814,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="106"/>
-      <c r="W6" s="106"/>
-      <c r="X6" s="106"/>
-      <c r="Y6" s="106"/>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="106"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="87"/>
+      <c r="U6" s="87"/>
+      <c r="V6" s="87"/>
+      <c r="W6" s="87"/>
+      <c r="X6" s="87"/>
+      <c r="Y6" s="87"/>
+      <c r="Z6" s="87"/>
+      <c r="AA6" s="87"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -2839,30 +2845,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="96"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="106"/>
-      <c r="AA7" s="106"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="87"/>
+      <c r="Z7" s="87"/>
+      <c r="AA7" s="87"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -2874,31 +2880,31 @@
       <c r="B8" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="106"/>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
+      <c r="X8" s="87"/>
+      <c r="Y8" s="87"/>
+      <c r="Z8" s="87"/>
+      <c r="AA8" s="87"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -2908,31 +2914,31 @@
     <row r="9" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="104"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="106"/>
-      <c r="AA9" s="106"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="87"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="87"/>
+      <c r="AA9" s="87"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -2952,21 +2958,21 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="106"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="106"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
-      <c r="T10" s="106"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="106"/>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="106"/>
-      <c r="AA10" s="106"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="87"/>
+      <c r="T10" s="87"/>
+      <c r="U10" s="87"/>
+      <c r="V10" s="87"/>
+      <c r="W10" s="87"/>
+      <c r="X10" s="87"/>
+      <c r="Y10" s="87"/>
+      <c r="Z10" s="87"/>
+      <c r="AA10" s="87"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -2988,21 +2994,21 @@
       <c r="J11" s="64"/>
       <c r="K11" s="65"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="106"/>
-      <c r="O11" s="106"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="106"/>
-      <c r="R11" s="106"/>
-      <c r="S11" s="106"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="106"/>
-      <c r="AA11" s="106"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
+      <c r="T11" s="87"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
+      <c r="Y11" s="87"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="87"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -3019,27 +3025,27 @@
       <c r="F12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="103" t="s">
-        <v>129</v>
-      </c>
-      <c r="J12" s="103"/>
-      <c r="K12" s="104"/>
+      <c r="I12" s="105" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" s="105"/>
+      <c r="K12" s="106"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
+      <c r="S12" s="87"/>
+      <c r="T12" s="87"/>
+      <c r="U12" s="87"/>
+      <c r="V12" s="87"/>
+      <c r="W12" s="87"/>
+      <c r="X12" s="87"/>
+      <c r="Y12" s="87"/>
+      <c r="Z12" s="87"/>
+      <c r="AA12" s="87"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
@@ -3054,25 +3060,25 @@
       <c r="F13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="103"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="104"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="106"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="106"/>
-      <c r="T13" s="106"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="106"/>
-      <c r="W13" s="106"/>
-      <c r="X13" s="106"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="106"/>
-      <c r="AA13" s="106"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="87"/>
+      <c r="T13" s="87"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="87"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
+      <c r="Y13" s="87"/>
+      <c r="Z13" s="87"/>
+      <c r="AA13" s="87"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
@@ -3088,25 +3094,25 @@
         <v>41</v>
       </c>
       <c r="G14" s="12"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="104"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="106"/>
       <c r="L14" s="10"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="106"/>
-      <c r="O14" s="106"/>
-      <c r="P14" s="106"/>
-      <c r="Q14" s="106"/>
-      <c r="R14" s="106"/>
-      <c r="S14" s="106"/>
-      <c r="T14" s="106"/>
-      <c r="U14" s="106"/>
-      <c r="V14" s="106"/>
-      <c r="W14" s="106"/>
-      <c r="X14" s="106"/>
-      <c r="Y14" s="106"/>
-      <c r="Z14" s="106"/>
-      <c r="AA14" s="106"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="87"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="87"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="87"/>
+      <c r="S14" s="87"/>
+      <c r="T14" s="87"/>
+      <c r="U14" s="87"/>
+      <c r="V14" s="87"/>
+      <c r="W14" s="87"/>
+      <c r="X14" s="87"/>
+      <c r="Y14" s="87"/>
+      <c r="Z14" s="87"/>
+      <c r="AA14" s="87"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
@@ -3122,9 +3128,9 @@
         <v>110</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="104"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="106"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
       <c r="N15" s="30"/>
@@ -3154,9 +3160,9 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="12"/>
-      <c r="I16" s="103"/>
-      <c r="J16" s="103"/>
-      <c r="K16" s="104"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="106"/>
       <c r="L16" s="35"/>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
@@ -3190,9 +3196,9 @@
         <v>42</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="103"/>
-      <c r="K17" s="104"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="106"/>
       <c r="L17" s="35"/>
       <c r="M17" s="35"/>
       <c r="N17" s="35"/>
@@ -3262,26 +3268,26 @@
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M19" s="35"/>
       <c r="N19" s="51"/>
       <c r="O19" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P19" s="35"/>
       <c r="Q19" s="52"/>
       <c r="R19" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T19" s="56"/>
       <c r="U19" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="V19" s="35"/>
       <c r="W19" s="58"/>
       <c r="X19" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Y19" s="67"/>
       <c r="Z19" s="35"/>
@@ -3302,23 +3308,23 @@
       <c r="J20" s="35"/>
       <c r="K20" s="49"/>
       <c r="L20" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M20" s="35"/>
       <c r="N20" s="55"/>
       <c r="O20" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P20" s="35"/>
       <c r="Q20" s="53"/>
       <c r="R20" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S20" s="35"/>
       <c r="V20" s="35"/>
       <c r="W20" s="59"/>
       <c r="X20" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y20" s="67"/>
       <c r="Z20" s="35"/>
@@ -3343,13 +3349,13 @@
       <c r="J21" s="35"/>
       <c r="K21" s="50"/>
       <c r="L21" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M21" s="35"/>
       <c r="P21" s="35"/>
       <c r="Q21" s="54"/>
       <c r="R21" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S21" s="35"/>
       <c r="T21" s="57"/>
@@ -3425,161 +3431,161 @@
       <c r="AF23" s="7"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="83" t="s">
+      <c r="A24" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="83"/>
-      <c r="C24" s="84" t="s">
+      <c r="B24" s="86"/>
+      <c r="C24" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="85"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="85"/>
-      <c r="K24" s="85"/>
-      <c r="L24" s="85"/>
-      <c r="M24" s="85"/>
-      <c r="N24" s="85"/>
-      <c r="O24" s="85"/>
-      <c r="P24" s="85"/>
-      <c r="Q24" s="85"/>
-      <c r="R24" s="85"/>
-      <c r="S24" s="85"/>
-      <c r="T24" s="85"/>
-      <c r="U24" s="85"/>
-      <c r="V24" s="85"/>
-      <c r="W24" s="85"/>
-      <c r="X24" s="85"/>
-      <c r="Y24" s="85"/>
-      <c r="Z24" s="85"/>
-      <c r="AA24" s="86"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="90"/>
+      <c r="O24" s="90"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="90"/>
+      <c r="R24" s="90"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="90"/>
+      <c r="U24" s="90"/>
+      <c r="V24" s="90"/>
+      <c r="W24" s="90"/>
+      <c r="X24" s="90"/>
+      <c r="Y24" s="90"/>
+      <c r="Z24" s="90"/>
+      <c r="AA24" s="91"/>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
-      <c r="C25" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="88"/>
-      <c r="J25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="88"/>
-      <c r="N25" s="88"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="88"/>
-      <c r="Q25" s="88"/>
-      <c r="R25" s="88"/>
-      <c r="S25" s="88"/>
-      <c r="T25" s="88"/>
-      <c r="U25" s="88"/>
-      <c r="V25" s="88"/>
-      <c r="W25" s="88"/>
-      <c r="X25" s="88"/>
-      <c r="Y25" s="88"/>
-      <c r="Z25" s="88"/>
-      <c r="AA25" s="89"/>
+      <c r="C25" s="92" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="93"/>
+      <c r="J25" s="93"/>
+      <c r="K25" s="93"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="93"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="93"/>
+      <c r="R25" s="93"/>
+      <c r="S25" s="93"/>
+      <c r="T25" s="93"/>
+      <c r="U25" s="93"/>
+      <c r="V25" s="93"/>
+      <c r="W25" s="93"/>
+      <c r="X25" s="93"/>
+      <c r="Y25" s="93"/>
+      <c r="Z25" s="93"/>
+      <c r="AA25" s="94"/>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="88"/>
-      <c r="T26" s="88"/>
-      <c r="U26" s="88"/>
-      <c r="V26" s="88"/>
-      <c r="W26" s="88"/>
-      <c r="X26" s="88"/>
-      <c r="Y26" s="88"/>
-      <c r="Z26" s="88"/>
-      <c r="AA26" s="89"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
+      <c r="I26" s="93"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="93"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="93"/>
+      <c r="N26" s="93"/>
+      <c r="O26" s="93"/>
+      <c r="P26" s="93"/>
+      <c r="Q26" s="93"/>
+      <c r="R26" s="93"/>
+      <c r="S26" s="93"/>
+      <c r="T26" s="93"/>
+      <c r="U26" s="93"/>
+      <c r="V26" s="93"/>
+      <c r="W26" s="93"/>
+      <c r="X26" s="93"/>
+      <c r="Y26" s="93"/>
+      <c r="Z26" s="93"/>
+      <c r="AA26" s="94"/>
     </row>
     <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="91"/>
-      <c r="N27" s="91"/>
-      <c r="O27" s="91"/>
-      <c r="P27" s="91"/>
-      <c r="Q27" s="91"/>
-      <c r="R27" s="91"/>
-      <c r="S27" s="91"/>
-      <c r="T27" s="91"/>
-      <c r="U27" s="91"/>
-      <c r="V27" s="91"/>
-      <c r="W27" s="91"/>
-      <c r="X27" s="91"/>
-      <c r="Y27" s="91"/>
-      <c r="Z27" s="91"/>
-      <c r="AA27" s="92"/>
+      <c r="C27" s="95" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="96"/>
+      <c r="J27" s="96"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="96"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="96"/>
+      <c r="O27" s="96"/>
+      <c r="P27" s="96"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="96"/>
+      <c r="S27" s="96"/>
+      <c r="T27" s="96"/>
+      <c r="U27" s="96"/>
+      <c r="V27" s="96"/>
+      <c r="W27" s="96"/>
+      <c r="X27" s="96"/>
+      <c r="Y27" s="96"/>
+      <c r="Z27" s="96"/>
+      <c r="AA27" s="97"/>
     </row>
     <row r="29" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="105" t="s">
+      <c r="A29" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="105"/>
-      <c r="L29" s="105"/>
-      <c r="M29" s="105"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="105"/>
-      <c r="P29" s="105"/>
-      <c r="Q29" s="105"/>
-      <c r="R29" s="105"/>
-      <c r="S29" s="105"/>
-      <c r="T29" s="105"/>
-      <c r="U29" s="105"/>
-      <c r="V29" s="105"/>
-      <c r="W29" s="105"/>
-      <c r="X29" s="105"/>
-      <c r="Y29" s="105"/>
-      <c r="Z29" s="105"/>
-      <c r="AA29" s="105"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="82"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="82"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="82"/>
+      <c r="R29" s="82"/>
+      <c r="S29" s="82"/>
+      <c r="T29" s="82"/>
+      <c r="U29" s="82"/>
+      <c r="V29" s="82"/>
+      <c r="W29" s="82"/>
+      <c r="X29" s="82"/>
+      <c r="Y29" s="82"/>
+      <c r="Z29" s="82"/>
+      <c r="AA29" s="82"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -4414,35 +4420,35 @@
       <c r="M55" s="10"/>
     </row>
     <row r="56" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="B56" s="105"/>
-      <c r="C56" s="105"/>
-      <c r="D56" s="105"/>
-      <c r="E56" s="105"/>
-      <c r="F56" s="105"/>
-      <c r="G56" s="105"/>
-      <c r="H56" s="105"/>
-      <c r="I56" s="105"/>
-      <c r="J56" s="105"/>
-      <c r="K56" s="105"/>
-      <c r="L56" s="105"/>
-      <c r="M56" s="105"/>
-      <c r="N56" s="105"/>
-      <c r="O56" s="105"/>
-      <c r="P56" s="105"/>
-      <c r="Q56" s="105"/>
-      <c r="R56" s="105"/>
-      <c r="S56" s="105"/>
-      <c r="T56" s="105"/>
-      <c r="U56" s="105"/>
-      <c r="V56" s="105"/>
-      <c r="W56" s="105"/>
-      <c r="X56" s="105"/>
-      <c r="Y56" s="105"/>
-      <c r="Z56" s="105"/>
-      <c r="AA56" s="105"/>
+      <c r="B56" s="82"/>
+      <c r="C56" s="82"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="82"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="82"/>
+      <c r="I56" s="82"/>
+      <c r="J56" s="82"/>
+      <c r="K56" s="82"/>
+      <c r="L56" s="82"/>
+      <c r="M56" s="82"/>
+      <c r="N56" s="82"/>
+      <c r="O56" s="82"/>
+      <c r="P56" s="82"/>
+      <c r="Q56" s="82"/>
+      <c r="R56" s="82"/>
+      <c r="S56" s="82"/>
+      <c r="T56" s="82"/>
+      <c r="U56" s="82"/>
+      <c r="V56" s="82"/>
+      <c r="W56" s="82"/>
+      <c r="X56" s="82"/>
+      <c r="Y56" s="82"/>
+      <c r="Z56" s="82"/>
+      <c r="AA56" s="82"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -5197,15 +5203,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A29:AA29"/>
-    <mergeCell ref="A56:AA56"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="M3:AA14"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:AA24"/>
@@ -5219,6 +5216,15 @@
     <mergeCell ref="C25:AA25"/>
     <mergeCell ref="C8:G9"/>
     <mergeCell ref="I12:K17"/>
+    <mergeCell ref="A29:AA29"/>
+    <mergeCell ref="A56:AA56"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="M3:AA14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5233,29 +5239,31 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:AA13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="13" width="9.140625" style="10"/>
+    <col min="2" max="11" width="9.140625" style="10"/>
+    <col min="12" max="12" width="10.5703125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -5274,35 +5282,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="96"/>
-      <c r="J3" s="83" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
+      <c r="J3" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -5310,35 +5318,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="96"/>
-      <c r="J4" s="83" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="J4" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
-      <c r="X4" s="106"/>
-      <c r="Y4" s="106"/>
-      <c r="Z4" s="106"/>
-      <c r="AA4" s="106"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -5347,26 +5355,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="93" t="s">
+      <c r="J5" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="106"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -5374,30 +5382,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="106"/>
-      <c r="W6" s="106"/>
-      <c r="X6" s="106"/>
-      <c r="Y6" s="106"/>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="106"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="87"/>
+      <c r="U6" s="87"/>
+      <c r="V6" s="87"/>
+      <c r="W6" s="87"/>
+      <c r="X6" s="87"/>
+      <c r="Y6" s="87"/>
+      <c r="Z6" s="87"/>
+      <c r="AA6" s="87"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -5405,30 +5413,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="96"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="106"/>
-      <c r="AA7" s="106"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="87"/>
+      <c r="Z7" s="87"/>
+      <c r="AA7" s="87"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -5440,31 +5448,31 @@
       <c r="B8" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="106"/>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
+      <c r="X8" s="87"/>
+      <c r="Y8" s="87"/>
+      <c r="Z8" s="87"/>
+      <c r="AA8" s="87"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -5474,31 +5482,31 @@
     <row r="9" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="104"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="106"/>
-      <c r="AA9" s="106"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="87"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="87"/>
+      <c r="AA9" s="87"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -5513,21 +5521,21 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="106"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="106"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
-      <c r="T10" s="106"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="106"/>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="106"/>
-      <c r="AA10" s="106"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="87"/>
+      <c r="T10" s="87"/>
+      <c r="U10" s="87"/>
+      <c r="V10" s="87"/>
+      <c r="W10" s="87"/>
+      <c r="X10" s="87"/>
+      <c r="Y10" s="87"/>
+      <c r="Z10" s="87"/>
+      <c r="AA10" s="87"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -5539,27 +5547,27 @@
       <c r="C11" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="96"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="106"/>
-      <c r="O11" s="106"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="106"/>
-      <c r="R11" s="106"/>
-      <c r="S11" s="106"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="106"/>
-      <c r="AA11" s="106"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="85"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
+      <c r="T11" s="87"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
+      <c r="Y11" s="87"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="87"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -5569,21 +5577,21 @@
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
+      <c r="S12" s="87"/>
+      <c r="T12" s="87"/>
+      <c r="U12" s="87"/>
+      <c r="V12" s="87"/>
+      <c r="W12" s="87"/>
+      <c r="X12" s="87"/>
+      <c r="Y12" s="87"/>
+      <c r="Z12" s="87"/>
+      <c r="AA12" s="87"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
@@ -5600,23 +5608,23 @@
       <c r="H13" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="J13" s="96"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="106"/>
-      <c r="T13" s="106"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="106"/>
-      <c r="W13" s="106"/>
-      <c r="X13" s="106"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="106"/>
-      <c r="AA13" s="106"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="85"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="87"/>
+      <c r="T13" s="87"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="87"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
+      <c r="Y13" s="87"/>
+      <c r="Z13" s="87"/>
+      <c r="AA13" s="87"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
@@ -5654,8 +5662,12 @@
       <c r="H15" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="94"/>
-      <c r="J15" s="96"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="113" t="s">
+        <v>146</v>
+      </c>
+      <c r="L15" s="19"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="13" t="s">
@@ -5665,17 +5677,11 @@
       <c r="H17" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="94"/>
-      <c r="J17" s="96"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
     <mergeCell ref="M3:AA13"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:G4"/>
@@ -5688,6 +5694,12 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G9"/>
     <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5711,20 +5723,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -5743,35 +5755,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="96"/>
-      <c r="J3" s="83" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
+      <c r="J3" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="87"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -5779,35 +5791,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="96"/>
-      <c r="J4" s="83" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="J4" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
-      <c r="X4" s="106"/>
-      <c r="Y4" s="106"/>
-      <c r="Z4" s="106"/>
-      <c r="AA4" s="106"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -5816,26 +5828,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="93" t="s">
+      <c r="J5" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="106"/>
-      <c r="Z5" s="106"/>
-      <c r="AA5" s="106"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -5843,30 +5855,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="106"/>
-      <c r="W6" s="106"/>
-      <c r="X6" s="106"/>
-      <c r="Y6" s="106"/>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="106"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="87"/>
+      <c r="U6" s="87"/>
+      <c r="V6" s="87"/>
+      <c r="W6" s="87"/>
+      <c r="X6" s="87"/>
+      <c r="Y6" s="87"/>
+      <c r="Z6" s="87"/>
+      <c r="AA6" s="87"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -5874,30 +5886,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="96"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="106"/>
-      <c r="AA7" s="106"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="87"/>
+      <c r="Z7" s="87"/>
+      <c r="AA7" s="87"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -5909,31 +5921,31 @@
       <c r="B8" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="106"/>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
+      <c r="X8" s="87"/>
+      <c r="Y8" s="87"/>
+      <c r="Z8" s="87"/>
+      <c r="AA8" s="87"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -5943,31 +5955,31 @@
     <row r="9" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="104"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-      <c r="Z9" s="106"/>
-      <c r="AA9" s="106"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="87"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
+      <c r="Y9" s="87"/>
+      <c r="Z9" s="87"/>
+      <c r="AA9" s="87"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -5982,21 +5994,21 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="106"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="106"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
-      <c r="T10" s="106"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="106"/>
-      <c r="Y10" s="106"/>
-      <c r="Z10" s="106"/>
-      <c r="AA10" s="106"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="87"/>
+      <c r="T10" s="87"/>
+      <c r="U10" s="87"/>
+      <c r="V10" s="87"/>
+      <c r="W10" s="87"/>
+      <c r="X10" s="87"/>
+      <c r="Y10" s="87"/>
+      <c r="Z10" s="87"/>
+      <c r="AA10" s="87"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -6012,21 +6024,21 @@
       <c r="F11" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="M11" s="106"/>
-      <c r="N11" s="106"/>
-      <c r="O11" s="106"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="106"/>
-      <c r="R11" s="106"/>
-      <c r="S11" s="106"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
-      <c r="Y11" s="106"/>
-      <c r="Z11" s="106"/>
-      <c r="AA11" s="106"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
+      <c r="T11" s="87"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
+      <c r="Y11" s="87"/>
+      <c r="Z11" s="87"/>
+      <c r="AA11" s="87"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -6041,21 +6053,21 @@
       <c r="F12" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
-      <c r="Y12" s="106"/>
-      <c r="Z12" s="106"/>
-      <c r="AA12" s="106"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
+      <c r="S12" s="87"/>
+      <c r="T12" s="87"/>
+      <c r="U12" s="87"/>
+      <c r="V12" s="87"/>
+      <c r="W12" s="87"/>
+      <c r="X12" s="87"/>
+      <c r="Y12" s="87"/>
+      <c r="Z12" s="87"/>
+      <c r="AA12" s="87"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
@@ -6074,21 +6086,21 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="106"/>
-      <c r="T13" s="106"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="106"/>
-      <c r="W13" s="106"/>
-      <c r="X13" s="106"/>
-      <c r="Y13" s="106"/>
-      <c r="Z13" s="106"/>
-      <c r="AA13" s="106"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="87"/>
+      <c r="T13" s="87"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="87"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
+      <c r="Y13" s="87"/>
+      <c r="Z13" s="87"/>
+      <c r="AA13" s="87"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
@@ -6189,161 +6201,161 @@
       <c r="AF16" s="7"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="83" t="s">
+      <c r="A17" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84" t="s">
+      <c r="B17" s="86"/>
+      <c r="C17" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="85"/>
-      <c r="K17" s="85"/>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="85"/>
-      <c r="Q17" s="85"/>
-      <c r="R17" s="85"/>
-      <c r="S17" s="85"/>
-      <c r="T17" s="85"/>
-      <c r="U17" s="85"/>
-      <c r="V17" s="85"/>
-      <c r="W17" s="85"/>
-      <c r="X17" s="85"/>
-      <c r="Y17" s="85"/>
-      <c r="Z17" s="85"/>
-      <c r="AA17" s="86"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="90"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="90"/>
+      <c r="AA17" s="91"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
-      <c r="C18" s="87" t="s">
+      <c r="C18" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="88"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="88"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-      <c r="T18" s="88"/>
-      <c r="U18" s="88"/>
-      <c r="V18" s="88"/>
-      <c r="W18" s="88"/>
-      <c r="X18" s="88"/>
-      <c r="Y18" s="88"/>
-      <c r="Z18" s="88"/>
-      <c r="AA18" s="89"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
+      <c r="M18" s="93"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="93"/>
+      <c r="Q18" s="93"/>
+      <c r="R18" s="93"/>
+      <c r="S18" s="93"/>
+      <c r="T18" s="93"/>
+      <c r="U18" s="93"/>
+      <c r="V18" s="93"/>
+      <c r="W18" s="93"/>
+      <c r="X18" s="93"/>
+      <c r="Y18" s="93"/>
+      <c r="Z18" s="93"/>
+      <c r="AA18" s="94"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="87" t="s">
+      <c r="C19" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="88"/>
-      <c r="R19" s="88"/>
-      <c r="S19" s="88"/>
-      <c r="T19" s="88"/>
-      <c r="U19" s="88"/>
-      <c r="V19" s="88"/>
-      <c r="W19" s="88"/>
-      <c r="X19" s="88"/>
-      <c r="Y19" s="88"/>
-      <c r="Z19" s="88"/>
-      <c r="AA19" s="89"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="93"/>
+      <c r="N19" s="93"/>
+      <c r="O19" s="93"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="93"/>
+      <c r="R19" s="93"/>
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="V19" s="93"/>
+      <c r="W19" s="93"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
+      <c r="Z19" s="93"/>
+      <c r="AA19" s="94"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
-      <c r="C20" s="90" t="s">
+      <c r="C20" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
-      <c r="P20" s="91"/>
-      <c r="Q20" s="91"/>
-      <c r="R20" s="91"/>
-      <c r="S20" s="91"/>
-      <c r="T20" s="91"/>
-      <c r="U20" s="91"/>
-      <c r="V20" s="91"/>
-      <c r="W20" s="91"/>
-      <c r="X20" s="91"/>
-      <c r="Y20" s="91"/>
-      <c r="Z20" s="91"/>
-      <c r="AA20" s="92"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="96"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="96"/>
+      <c r="R20" s="96"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="96"/>
+      <c r="U20" s="96"/>
+      <c r="V20" s="96"/>
+      <c r="W20" s="96"/>
+      <c r="X20" s="96"/>
+      <c r="Y20" s="96"/>
+      <c r="Z20" s="96"/>
+      <c r="AA20" s="97"/>
     </row>
     <row r="22" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="105"/>
-      <c r="J22" s="105"/>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="105"/>
-      <c r="N22" s="105"/>
-      <c r="O22" s="105"/>
-      <c r="P22" s="105"/>
-      <c r="Q22" s="105"/>
-      <c r="R22" s="105"/>
-      <c r="S22" s="105"/>
-      <c r="T22" s="105"/>
-      <c r="U22" s="105"/>
-      <c r="V22" s="105"/>
-      <c r="W22" s="105"/>
-      <c r="X22" s="105"/>
-      <c r="Y22" s="105"/>
-      <c r="Z22" s="105"/>
-      <c r="AA22" s="105"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="82"/>
+      <c r="W22" s="82"/>
+      <c r="X22" s="82"/>
+      <c r="Y22" s="82"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="82"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -7142,35 +7154,35 @@
       <c r="J46" s="19"/>
     </row>
     <row r="49" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="105" t="s">
+      <c r="A49" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="105"/>
-      <c r="C49" s="105"/>
-      <c r="D49" s="105"/>
-      <c r="E49" s="105"/>
-      <c r="F49" s="105"/>
-      <c r="G49" s="105"/>
-      <c r="H49" s="105"/>
-      <c r="I49" s="105"/>
-      <c r="J49" s="105"/>
-      <c r="K49" s="105"/>
-      <c r="L49" s="105"/>
-      <c r="M49" s="105"/>
-      <c r="N49" s="105"/>
-      <c r="O49" s="105"/>
-      <c r="P49" s="105"/>
-      <c r="Q49" s="105"/>
-      <c r="R49" s="105"/>
-      <c r="S49" s="105"/>
-      <c r="T49" s="105"/>
-      <c r="U49" s="105"/>
-      <c r="V49" s="105"/>
-      <c r="W49" s="105"/>
-      <c r="X49" s="105"/>
-      <c r="Y49" s="105"/>
-      <c r="Z49" s="105"/>
-      <c r="AA49" s="105"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="82"/>
+      <c r="O49" s="82"/>
+      <c r="P49" s="82"/>
+      <c r="Q49" s="82"/>
+      <c r="R49" s="82"/>
+      <c r="S49" s="82"/>
+      <c r="T49" s="82"/>
+      <c r="U49" s="82"/>
+      <c r="V49" s="82"/>
+      <c r="W49" s="82"/>
+      <c r="X49" s="82"/>
+      <c r="Y49" s="82"/>
+      <c r="Z49" s="82"/>
+      <c r="AA49" s="82"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -7917,16 +7929,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:AA13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="C19:AA19"/>
     <mergeCell ref="C20:AA20"/>
     <mergeCell ref="A22:AA22"/>
@@ -7938,6 +7940,16 @@
     <mergeCell ref="C17:AA17"/>
     <mergeCell ref="C18:AA18"/>
     <mergeCell ref="C8:G9"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:AA13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7961,20 +7973,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -7990,32 +8002,32 @@
       <c r="AC2" s="7"/>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="83"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="96"/>
-      <c r="J3" s="83" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="85"/>
+      <c r="J3" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
-      <c r="X3" s="106"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="R3" s="87"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
@@ -8023,32 +8035,32 @@
       <c r="AC3" s="7"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="96"/>
-      <c r="J4" s="83" t="s">
+      <c r="B4" s="86"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="J4" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
-      <c r="X4" s="106"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
@@ -8057,21 +8069,21 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
@@ -8079,27 +8091,27 @@
       <c r="AC5" s="7"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="96"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="106"/>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="106"/>
-      <c r="W6" s="106"/>
-      <c r="X6" s="106"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="87"/>
+      <c r="U6" s="87"/>
+      <c r="V6" s="87"/>
+      <c r="W6" s="87"/>
+      <c r="X6" s="87"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
@@ -8107,27 +8119,27 @@
       <c r="AC6" s="7"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="96"/>
-      <c r="M7" s="106"/>
-      <c r="N7" s="106"/>
-      <c r="O7" s="106"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
@@ -8139,28 +8151,28 @@
       <c r="B8" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="97"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="35"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="106"/>
-      <c r="O8" s="106"/>
-      <c r="P8" s="106"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="106"/>
-      <c r="W8" s="106"/>
-      <c r="X8" s="106"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
+      <c r="X8" s="87"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
@@ -8170,28 +8182,28 @@
     <row r="9" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="104"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="106"/>
-      <c r="O9" s="106"/>
-      <c r="P9" s="106"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="87"/>
+      <c r="U9" s="87"/>
+      <c r="V9" s="87"/>
+      <c r="W9" s="87"/>
+      <c r="X9" s="87"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
@@ -8206,18 +8218,18 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="106"/>
-      <c r="O10" s="106"/>
-      <c r="P10" s="106"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
-      <c r="T10" s="106"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="106"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="87"/>
+      <c r="T10" s="87"/>
+      <c r="U10" s="87"/>
+      <c r="V10" s="87"/>
+      <c r="W10" s="87"/>
+      <c r="X10" s="87"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
@@ -8233,18 +8245,18 @@
       <c r="F11" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="M11" s="106"/>
-      <c r="N11" s="106"/>
-      <c r="O11" s="106"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="106"/>
-      <c r="R11" s="106"/>
-      <c r="S11" s="106"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="106"/>
-      <c r="W11" s="106"/>
-      <c r="X11" s="106"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
+      <c r="T11" s="87"/>
+      <c r="U11" s="87"/>
+      <c r="V11" s="87"/>
+      <c r="W11" s="87"/>
+      <c r="X11" s="87"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
@@ -8259,18 +8271,18 @@
       <c r="F12" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="106"/>
-      <c r="W12" s="106"/>
-      <c r="X12" s="106"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
+      <c r="S12" s="87"/>
+      <c r="T12" s="87"/>
+      <c r="U12" s="87"/>
+      <c r="V12" s="87"/>
+      <c r="W12" s="87"/>
+      <c r="X12" s="87"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
@@ -8287,18 +8299,18 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="106"/>
-      <c r="O13" s="106"/>
-      <c r="P13" s="106"/>
-      <c r="Q13" s="106"/>
-      <c r="R13" s="106"/>
-      <c r="S13" s="106"/>
-      <c r="T13" s="106"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="106"/>
-      <c r="W13" s="106"/>
-      <c r="X13" s="106"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
+      <c r="S13" s="87"/>
+      <c r="T13" s="87"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="87"/>
+      <c r="W13" s="87"/>
+      <c r="X13" s="87"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
@@ -8324,124 +8336,124 @@
       <c r="AC14" s="7"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="83"/>
-      <c r="C15" s="84" t="s">
+      <c r="B15" s="86"/>
+      <c r="C15" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="85"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="85"/>
-      <c r="K15" s="85"/>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="85"/>
-      <c r="P15" s="85"/>
-      <c r="Q15" s="85"/>
-      <c r="R15" s="85"/>
-      <c r="S15" s="85"/>
-      <c r="T15" s="85"/>
-      <c r="U15" s="85"/>
-      <c r="V15" s="85"/>
-      <c r="W15" s="85"/>
-      <c r="X15" s="86"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="90"/>
+      <c r="Q15" s="90"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="90"/>
+      <c r="T15" s="90"/>
+      <c r="U15" s="90"/>
+      <c r="V15" s="90"/>
+      <c r="W15" s="90"/>
+      <c r="X15" s="91"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="88"/>
-      <c r="U16" s="88"/>
-      <c r="V16" s="88"/>
-      <c r="W16" s="88"/>
-      <c r="X16" s="89"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="93"/>
+      <c r="W16" s="93"/>
+      <c r="X16" s="94"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
-      <c r="C17" s="90" t="s">
+      <c r="C17" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="91"/>
-      <c r="M17" s="91"/>
-      <c r="N17" s="91"/>
-      <c r="O17" s="91"/>
-      <c r="P17" s="91"/>
-      <c r="Q17" s="91"/>
-      <c r="R17" s="91"/>
-      <c r="S17" s="91"/>
-      <c r="T17" s="91"/>
-      <c r="U17" s="91"/>
-      <c r="V17" s="91"/>
-      <c r="W17" s="91"/>
-      <c r="X17" s="92"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="96"/>
+      <c r="O17" s="96"/>
+      <c r="P17" s="96"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="96"/>
+      <c r="S17" s="96"/>
+      <c r="T17" s="96"/>
+      <c r="U17" s="96"/>
+      <c r="V17" s="96"/>
+      <c r="W17" s="96"/>
+      <c r="X17" s="97"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C19" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110" t="s">
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111" t="s">
         <v>106</v>
       </c>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110" t="s">
-        <v>145</v>
-      </c>
-      <c r="J19" s="110"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" s="111"/>
       <c r="K19" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="L19" s="110" t="s">
+      <c r="L19" s="111" t="s">
+        <v>142</v>
+      </c>
+      <c r="M19" s="111"/>
+      <c r="N19" s="111" t="s">
         <v>144</v>
       </c>
-      <c r="M19" s="110"/>
-      <c r="N19" s="110" t="s">
-        <v>146</v>
-      </c>
-      <c r="O19" s="110"/>
-      <c r="P19" s="110" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q19" s="110"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="111" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q19" s="111"/>
       <c r="R19" s="108" t="s">
         <v>108</v>
       </c>
@@ -8456,193 +8468,251 @@
       <c r="B20" s="10">
         <v>1</v>
       </c>
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
-      <c r="G20" s="109"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
       <c r="K20" s="38"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109"/>
-      <c r="N20" s="111"/>
-      <c r="O20" s="111"/>
-      <c r="P20" s="111"/>
-      <c r="Q20" s="111"/>
-      <c r="R20" s="112"/>
-      <c r="S20" s="112"/>
-      <c r="T20" s="112"/>
-      <c r="U20" s="112"/>
-      <c r="V20" s="112"/>
-      <c r="W20" s="112"/>
-      <c r="X20" s="112"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="112"/>
+      <c r="O20" s="112"/>
+      <c r="P20" s="112"/>
+      <c r="Q20" s="112"/>
+      <c r="R20" s="109"/>
+      <c r="S20" s="109"/>
+      <c r="T20" s="109"/>
+      <c r="U20" s="109"/>
+      <c r="V20" s="109"/>
+      <c r="W20" s="109"/>
+      <c r="X20" s="109"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>2</v>
       </c>
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="109"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
       <c r="K21" s="38"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="109"/>
-      <c r="O21" s="109"/>
-      <c r="P21" s="109"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="107"/>
-      <c r="S21" s="107"/>
-      <c r="T21" s="107"/>
-      <c r="U21" s="107"/>
-      <c r="V21" s="107"/>
-      <c r="W21" s="107"/>
-      <c r="X21" s="107"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="107"/>
+      <c r="N21" s="107"/>
+      <c r="O21" s="107"/>
+      <c r="P21" s="107"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="110"/>
+      <c r="S21" s="110"/>
+      <c r="T21" s="110"/>
+      <c r="U21" s="110"/>
+      <c r="V21" s="110"/>
+      <c r="W21" s="110"/>
+      <c r="X21" s="110"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>3</v>
       </c>
-      <c r="C22" s="109"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="107"/>
+      <c r="I22" s="107"/>
+      <c r="J22" s="107"/>
       <c r="K22" s="38"/>
-      <c r="L22" s="109"/>
-      <c r="M22" s="109"/>
-      <c r="N22" s="109"/>
-      <c r="O22" s="109"/>
-      <c r="P22" s="109"/>
-      <c r="Q22" s="109"/>
-      <c r="R22" s="107"/>
-      <c r="S22" s="107"/>
-      <c r="T22" s="107"/>
-      <c r="U22" s="107"/>
-      <c r="V22" s="107"/>
-      <c r="W22" s="107"/>
-      <c r="X22" s="107"/>
+      <c r="L22" s="107"/>
+      <c r="M22" s="107"/>
+      <c r="N22" s="107"/>
+      <c r="O22" s="107"/>
+      <c r="P22" s="107"/>
+      <c r="Q22" s="107"/>
+      <c r="R22" s="110"/>
+      <c r="S22" s="110"/>
+      <c r="T22" s="110"/>
+      <c r="U22" s="110"/>
+      <c r="V22" s="110"/>
+      <c r="W22" s="110"/>
+      <c r="X22" s="110"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>4</v>
       </c>
-      <c r="C23" s="109"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="107"/>
       <c r="K23" s="38"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="109"/>
-      <c r="P23" s="109"/>
-      <c r="Q23" s="109"/>
-      <c r="R23" s="107"/>
-      <c r="S23" s="107"/>
-      <c r="T23" s="107"/>
-      <c r="U23" s="107"/>
-      <c r="V23" s="107"/>
-      <c r="W23" s="107"/>
-      <c r="X23" s="107"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="107"/>
+      <c r="O23" s="107"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="110"/>
+      <c r="T23" s="110"/>
+      <c r="U23" s="110"/>
+      <c r="V23" s="110"/>
+      <c r="W23" s="110"/>
+      <c r="X23" s="110"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>5</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="109"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="107"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="107"/>
+      <c r="J24" s="107"/>
       <c r="K24" s="38"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109"/>
-      <c r="N24" s="109"/>
-      <c r="O24" s="109"/>
-      <c r="P24" s="109"/>
-      <c r="Q24" s="109"/>
-      <c r="R24" s="107"/>
-      <c r="S24" s="107"/>
-      <c r="T24" s="107"/>
-      <c r="U24" s="107"/>
-      <c r="V24" s="107"/>
-      <c r="W24" s="107"/>
-      <c r="X24" s="107"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="107"/>
+      <c r="O24" s="107"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="107"/>
+      <c r="R24" s="110"/>
+      <c r="S24" s="110"/>
+      <c r="T24" s="110"/>
+      <c r="U24" s="110"/>
+      <c r="V24" s="110"/>
+      <c r="W24" s="110"/>
+      <c r="X24" s="110"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>6</v>
       </c>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
-      <c r="J25" s="109"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="107"/>
+      <c r="J25" s="107"/>
       <c r="K25" s="38"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="109"/>
-      <c r="O25" s="109"/>
-      <c r="P25" s="109"/>
-      <c r="Q25" s="109"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
-      <c r="U25" s="107"/>
-      <c r="V25" s="107"/>
-      <c r="W25" s="107"/>
-      <c r="X25" s="107"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="107"/>
+      <c r="O25" s="107"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="110"/>
+      <c r="S25" s="110"/>
+      <c r="T25" s="110"/>
+      <c r="U25" s="110"/>
+      <c r="V25" s="110"/>
+      <c r="W25" s="110"/>
+      <c r="X25" s="110"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="109"/>
+      <c r="C26" s="107"/>
+      <c r="D26" s="107"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="107"/>
+      <c r="J26" s="107"/>
       <c r="K26" s="38"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="109"/>
-      <c r="O26" s="109"/>
-      <c r="P26" s="109"/>
-      <c r="Q26" s="109"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
-      <c r="U26" s="107"/>
-      <c r="V26" s="107"/>
-      <c r="W26" s="107"/>
-      <c r="X26" s="107"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="107"/>
+      <c r="N26" s="107"/>
+      <c r="O26" s="107"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="110"/>
+      <c r="S26" s="110"/>
+      <c r="T26" s="110"/>
+      <c r="U26" s="110"/>
+      <c r="V26" s="110"/>
+      <c r="W26" s="110"/>
+      <c r="X26" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C16:X16"/>
+    <mergeCell ref="C17:X17"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C15:X15"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:X13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C8:G9"/>
     <mergeCell ref="P24:Q24"/>
     <mergeCell ref="P25:Q25"/>
     <mergeCell ref="P26:Q26"/>
@@ -8659,64 +8729,6 @@
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="P22:Q22"/>
     <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:X13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C8:G9"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C16:X16"/>
-    <mergeCell ref="C17:X17"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C15:X15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>